<commit_message>
updated images and database tutorial section 2
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-02.data.xlsx
+++ b/artifact/data/rdbms-02.data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10120"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,16 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="-20560" windowWidth="33600" windowHeight="10280" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="12540" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
     <sheet name="DynamicSQL1" sheetId="3" r:id="rId2"/>
     <sheet name="DynamicSQL1a" sheetId="5" r:id="rId3"/>
-    <sheet name="db2_payroll_batch" sheetId="4" r:id="rId4"/>
+    <sheet name="DynamicSQL2" sheetId="6" r:id="rId4"/>
+    <sheet name="DynamicSQL2a" sheetId="7" r:id="rId5"/>
+    <sheet name="DynamicSQL3" sheetId="8" r:id="rId6"/>
+    <sheet name="db2_payroll_batch" sheetId="4" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -51,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t>true</t>
   </si>
@@ -164,6 +167,285 @@
         <family val="1"/>
       </rPr>
       <t>${customer country}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>'
+ORDER BY REP_NAME, CUSTOMER_NAME;</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT
+	A.TITLE,
+	C.NAME,
+	R.NAME,
+	UNITPRICE
+FROM TRACKS C, ALBUMS A, ARTISTS R
+WHERE C.ALBUMID = A.ALBUMID
+      AND A.ARTISTID = R.ARTISTID</t>
+  </si>
+  <si>
+    <t>songs SQL</t>
+  </si>
+  <si>
+    <t>mediatype where clause</t>
+  </si>
+  <si>
+    <r>
+      <t>AND C.MEDIATYPEID IN (SELECT MEDIATYPEID FROM MEDIA_TYPES WHERE NAME LIKE '%</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${media type}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>%')</t>
+    </r>
+  </si>
+  <si>
+    <t>genre where clause</t>
+  </si>
+  <si>
+    <r>
+      <t>AND C.GENREID IN (SELECT GENREID FROM GENRES WHERE NAME LIKE '%</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${genre}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>%')</t>
+    </r>
+  </si>
+  <si>
+    <t>album where clause</t>
+  </si>
+  <si>
+    <r>
+      <t>AND C.ALBUMID IN (SELECT B.ALBUMID FROM ALBUMS B WHERE TITLE LIKE '%</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${album}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>%')</t>
+    </r>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>Jazz</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <r>
+      <t>$(syspath|out|fullpath)/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${media type}${genre}${album}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>.csv</t>
+    </r>
+  </si>
+  <si>
+    <t>genre output</t>
+  </si>
+  <si>
+    <t>mediatype output</t>
+  </si>
+  <si>
+    <t>album output</t>
+  </si>
+  <si>
+    <r>
+      <t>$(syspath|out|fullpath)/MEDIA-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${media type}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>.csv</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>$(syspath|out|fullpath)/GENRE-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${genre}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>.csv</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>$(syspath|out|fullpath)/ALBUM-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${album}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>.csv</t>
+    </r>
+  </si>
+  <si>
+    <t>songs detailed SELECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	,
+	COMPOSER, MILLISECONDS / 1000 AS SONG_LENGTH_SEC,
+	(BYTES / 1024) AS SONG_SIZE_KB,
+	(SELECT NAME FROM GENRES G WHERE G.GENREID = C.GENREID) AS GENRE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT
+	A.TITLE,
+	C.NAME,
+	R.NAME,
+	UNITPRICE
+	</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${detailed select clause}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+FROM TRACKS C, ALBUMS A, ARTISTS R
+WHERE C.ALBUMID = A.ALBUMID
+      AND A.ARTISTID = R.ARTISTID
+      AND C.GENREID IN (SELECT GENREID FROM GENRES WHERE NAME LIKE '%Jazz%')</t>
+    </r>
+  </si>
+  <si>
+    <t>$(syspath|out|fullpath)/output.csv</t>
+  </si>
+  <si>
+    <t>mydb.treatNullAs</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>customercountry</t>
+  </si>
+  <si>
+    <r>
+      <t>SELECT
+	C.COMPANY                        AS CUSTOMER_COMPANY,
+	C.FIRSTNAME || ' ' || C.LASTNAME AS CUSTOMER_NAME,
+	C.EMAIL                          AS CUSTOMER_EMAIL,
+	E.TITLE                          AS REP_TITLE,
+	E.FIRSTNAME || ' ' || E.LASTNAME AS REP_NAME,
+	E.EMAIL                          AS REP_EMAIL
+FROM customers C, employees E
+WHERE
+	C.SUPPORTREPID = E.EMPLOYEEID AND
+	C.COUNTRY = '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${customercountry}</t>
     </r>
     <r>
       <rPr>
@@ -384,7 +666,917 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="94">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -993,7 +2185,7 @@
   <dimension ref="A1:AAA24"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A8" sqref="A8:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1188,37 +2380,37 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="23" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="93" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="92" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="21" priority="7" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="91" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B7 B13:B1048576">
-    <cfRule type="expression" dxfId="20" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="8" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="19" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="89" priority="9">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="18" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="17" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="expression" dxfId="16" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1232,7 +2424,7 @@
   <dimension ref="A1:AAA24"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1249,7 +2441,7 @@
         <v>26</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C1" s="7"/>
       <c r="HA1" s="6"/>
@@ -1257,7 +2449,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="12" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>28</v>
@@ -1394,21 +2586,21 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="84" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="83" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1421,7 +2613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D8DAAF-5FA2-3F45-9587-0BF4D1FC794A}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1584,21 +2776,21 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="79" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="78" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1608,6 +2800,849 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A45AD1-9E5F-1D4C-908D-A0E650034FFE}">
+  <dimension ref="A1:AAA24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="111.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703" ht="136">
+      <c r="A1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703">
+      <c r="A2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="A3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="A4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="A5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="A6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="7"/>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="7"/>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="7"/>
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="7"/>
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:703">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A1:A4 A9:A1048576 A7">
+    <cfRule type="beginsWith" dxfId="74" priority="16" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="73" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="72" priority="18" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B4 B9:B1048576 B7">
+    <cfRule type="expression" dxfId="71" priority="19" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="70" priority="20">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="beginsWith" dxfId="69" priority="11" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A8,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="68" priority="12" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A8,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="67" priority="13" stopIfTrue="1">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="66" priority="14" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="65" priority="15">
+      <formula>LEN(TRIM(B8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="beginsWith" dxfId="64" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A5,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="63" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A5,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="62" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="61" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="60" priority="10">
+      <formula>LEN(TRIM(B5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="beginsWith" dxfId="59" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="58" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="57" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="expression" dxfId="56" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="55" priority="5">
+      <formula>LEN(TRIM(B6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5615C66-E964-DF4A-B5AC-E5F1CF42C1A0}">
+  <dimension ref="A1:AAA24"/>
+  <sheetViews>
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703" ht="136">
+      <c r="A1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703">
+      <c r="A2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="A3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="A4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="A5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="A6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="A7" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="7"/>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="7"/>
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="7"/>
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:703">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A1:A4 A9:A1048576">
+    <cfRule type="beginsWith" dxfId="54" priority="26" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="53" priority="27" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="52" priority="28" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B4 B9:B1048576">
+    <cfRule type="expression" dxfId="51" priority="29" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="50" priority="30">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="beginsWith" dxfId="49" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A8,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="48" priority="22" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A8,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="47" priority="23" stopIfTrue="1">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="46" priority="24" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="45" priority="25">
+      <formula>LEN(TRIM(B8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="beginsWith" dxfId="44" priority="16" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A5,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="43" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A5,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="42" priority="18" stopIfTrue="1">
+      <formula>LEN(TRIM(A5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="41" priority="19" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="40" priority="20">
+      <formula>LEN(TRIM(B5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="beginsWith" dxfId="39" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="38" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="37" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="expression" dxfId="36" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="35" priority="10">
+      <formula>LEN(TRIM(B6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="beginsWith" dxfId="34" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A7,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="33" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A7,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="32" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="expression" dxfId="31" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="30" priority="5">
+      <formula>LEN(TRIM(B7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36E0F6B-8C25-A04E-A958-58437CE8DA7B}">
+  <dimension ref="A1:AAA24"/>
+  <sheetViews>
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="93.5" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703" ht="170">
+      <c r="A1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703" ht="68">
+      <c r="A2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="A3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="A4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="A5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="A6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="A7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="A9" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="7"/>
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:703">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A1:A4 A9:A1048576">
+    <cfRule type="beginsWith" dxfId="29" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="28" priority="22" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="27" priority="23" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B4 B9:B1048576">
+    <cfRule type="expression" dxfId="26" priority="24" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="25" priority="25">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="beginsWith" dxfId="24" priority="16" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A8,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="23" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A8,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="22" priority="18" stopIfTrue="1">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="21" priority="19" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="20" priority="20">
+      <formula>LEN(TRIM(B8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="beginsWith" dxfId="19" priority="11" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A5,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="18" priority="12" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A5,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="17" priority="13" stopIfTrue="1">
+      <formula>LEN(TRIM(A5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="15" priority="15">
+      <formula>LEN(TRIM(B5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="beginsWith" dxfId="14" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="13" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="12" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="10" priority="10">
+      <formula>LEN(TRIM(B6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A7,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A7,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="7" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
+      <formula>LEN(TRIM(B7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEF39D-E984-C449-9030-77DFE4612593}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>

</xml_diff>

<commit_message>
complete Section 2 of Database Automation tutorial
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-02.data.xlsx
+++ b/artifact/data/rdbms-02.data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10120"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10124"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="12540" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="12540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
   <si>
     <t>true</t>
   </si>
@@ -456,6 +456,12 @@
       <t>'
 ORDER BY REP_NAME, CUSTOMER_NAME;</t>
     </r>
+  </si>
+  <si>
+    <t>media type</t>
+  </si>
+  <si>
+    <t>${mediatype}</t>
   </si>
 </sst>
 </file>
@@ -2803,7 +2809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A45AD1-9E5F-1D4C-908D-A0E650034FFE}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3066,14 +3072,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5615C66-E964-DF4A-B5AC-E5F1CF42C1A0}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="23.83203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="111.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
@@ -3157,8 +3163,12 @@
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>58</v>
+      </c>
       <c r="C8" s="7"/>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>

</xml_diff>

<commit_message>
updates section 2 of Database Automation
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-02.data.xlsx
+++ b/artifact/data/rdbms-02.data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10124"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="12540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2740" yWindow="1320" windowWidth="33600" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -18,10 +18,9 @@
     <sheet name="DynamicSQL2" sheetId="6" r:id="rId4"/>
     <sheet name="DynamicSQL2a" sheetId="7" r:id="rId5"/>
     <sheet name="DynamicSQL3" sheetId="8" r:id="rId6"/>
-    <sheet name="db2_payroll_batch" sheetId="4" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>true</t>
   </si>
@@ -93,24 +92,6 @@
   </si>
   <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>client</t>
-  </si>
-  <si>
-    <t>select * from db2.payroll_batch where CLIENT_ID = ${client}</t>
-  </si>
-  <si>
-    <t>39832</t>
-  </si>
-  <si>
-    <t>my baseline</t>
-  </si>
-  <si>
-    <t>$(syspath|data|fullpath)/baseline.csv</t>
-  </si>
-  <si>
-    <t>my_db2 select1</t>
   </si>
   <si>
     <t>mydb.type</t>
@@ -672,72 +653,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="94">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="89">
     <dxf>
       <font>
         <b val="0"/>
@@ -2190,8 +2106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B12"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -2275,10 +2191,10 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" s="7"/>
       <c r="HA8" s="4"/>
@@ -2286,10 +2202,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C9" s="7"/>
       <c r="HA9" s="4"/>
@@ -2297,10 +2213,10 @@
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C10" s="7"/>
       <c r="HA10" s="4"/>
@@ -2308,16 +2224,16 @@
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>0</v>
@@ -2386,37 +2302,37 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="93" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="88" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="92" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="87" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="91" priority="7" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="86" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B7 B13:B1048576">
-    <cfRule type="expression" dxfId="90" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="8" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="89" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="84" priority="9">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="88" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="87" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="expression" dxfId="86" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="85" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2444,10 +2360,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="204">
       <c r="A1" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C1" s="7"/>
       <c r="HA1" s="6"/>
@@ -2455,10 +2371,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C2" s="7"/>
       <c r="HA2" s="6"/>
@@ -2592,21 +2508,21 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="84" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="79" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="83" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="78" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="82" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="81" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="80" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2634,10 +2550,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="204">
       <c r="A1" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" s="7"/>
       <c r="HA1" s="6"/>
@@ -2645,10 +2561,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="12" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C2" s="7"/>
       <c r="HA2" s="6"/>
@@ -2782,21 +2698,21 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="79" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="74" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="78" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="73" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="77" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="76" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="75" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2824,10 +2740,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="136">
       <c r="A1" s="12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C1" s="7"/>
       <c r="HA1" s="6"/>
@@ -2835,10 +2751,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7"/>
       <c r="HA2" s="6"/>
@@ -2846,10 +2762,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C3" s="7"/>
       <c r="HA3" s="6"/>
@@ -2857,10 +2773,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C4" s="7"/>
       <c r="HA4" s="4"/>
@@ -2868,10 +2784,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C5" s="7"/>
       <c r="HA5" s="4"/>
@@ -2879,10 +2795,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C6" s="7"/>
       <c r="HA6" s="4"/>
@@ -2988,78 +2904,78 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A4 A9:A1048576 A7">
-    <cfRule type="beginsWith" dxfId="74" priority="16" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="69" priority="16" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="73" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="68" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="72" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B4 B9:B1048576 B7">
-    <cfRule type="expression" dxfId="71" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="70" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="20">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="beginsWith" dxfId="69" priority="11" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="64" priority="11" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A8,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="68" priority="12" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="63" priority="12" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A8,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="67" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="66" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="65" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="15">
       <formula>LEN(TRIM(B8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="beginsWith" dxfId="64" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="59" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A5,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="63" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="58" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A5,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="62" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="61" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="60" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="10">
       <formula>LEN(TRIM(B5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="beginsWith" dxfId="59" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="54" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="58" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="53" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="57" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="56" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="55" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="5">
       <formula>LEN(TRIM(B6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3072,7 +2988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5615C66-E964-DF4A-B5AC-E5F1CF42C1A0}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -3087,10 +3003,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="136">
       <c r="A1" s="12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C1" s="7"/>
       <c r="HA1" s="6"/>
@@ -3098,10 +3014,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7"/>
       <c r="HA2" s="6"/>
@@ -3109,10 +3025,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C3" s="7"/>
       <c r="HA3" s="6"/>
@@ -3120,10 +3036,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C4" s="7"/>
       <c r="HA4" s="4"/>
@@ -3131,10 +3047,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="12" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C5" s="7"/>
       <c r="HA5" s="4"/>
@@ -3142,10 +3058,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C6" s="7"/>
       <c r="HA6" s="4"/>
@@ -3153,10 +3069,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C7" s="7"/>
       <c r="HA7" s="4"/>
@@ -3164,10 +3080,10 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="12" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C8" s="7"/>
       <c r="HA8" s="4"/>
@@ -3259,97 +3175,97 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A4 A9:A1048576">
-    <cfRule type="beginsWith" dxfId="54" priority="26" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="49" priority="26" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="53" priority="27" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="48" priority="27" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="52" priority="28" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B4 B9:B1048576">
-    <cfRule type="expression" dxfId="51" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="29" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="50" priority="30">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="30">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="beginsWith" dxfId="49" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="44" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A8,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="22" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="43" priority="22" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A8,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="47" priority="23" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="23" stopIfTrue="1">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="46" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="24" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="45" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="25">
       <formula>LEN(TRIM(B8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="beginsWith" dxfId="44" priority="16" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="39" priority="16" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A5,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="43" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="38" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A5,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="42" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="41" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="40" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="20">
       <formula>LEN(TRIM(B5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="beginsWith" dxfId="39" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="34" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="33" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="37" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="36" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="35" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="10">
       <formula>LEN(TRIM(B6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="beginsWith" dxfId="34" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="29" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A7,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="33" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="28" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A7,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="32" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="31" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="30" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="5">
       <formula>LEN(TRIM(B7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3363,13 +3279,13 @@
   <dimension ref="A1:AAA24"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="93.5" style="2" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="92.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
@@ -3377,10 +3293,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="170">
       <c r="A1" s="12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C1" s="7"/>
       <c r="HA1" s="6"/>
@@ -3388,10 +3304,10 @@
     </row>
     <row r="2" spans="1:703" ht="68">
       <c r="A2" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C2" s="7"/>
       <c r="HA2" s="6"/>
@@ -3399,10 +3315,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C3" s="7"/>
       <c r="HA3" s="6"/>
@@ -3410,10 +3326,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C4" s="7"/>
       <c r="HA4" s="4"/>
@@ -3421,10 +3337,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C5" s="7"/>
       <c r="HA5" s="4"/>
@@ -3432,10 +3348,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" s="7"/>
       <c r="HA6" s="4"/>
@@ -3443,10 +3359,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C7" s="7"/>
       <c r="HA7" s="4"/>
@@ -3454,7 +3370,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>0</v>
@@ -3465,10 +3381,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C9" s="7"/>
       <c r="HA9" s="4"/>
@@ -3553,290 +3469,98 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A4 A9:A1048576">
-    <cfRule type="beginsWith" dxfId="29" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="24" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="22" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="23" priority="22" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="27" priority="23" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="23" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B4 B9:B1048576">
-    <cfRule type="expression" dxfId="26" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="25" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="25">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="beginsWith" dxfId="24" priority="16" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="19" priority="16" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A8,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="23" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="18" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A8,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="22" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="21" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="20">
       <formula>LEN(TRIM(B8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="beginsWith" dxfId="19" priority="11" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="14" priority="11" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A5,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="12" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="13" priority="12" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A5,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="17" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="15">
       <formula>LEN(TRIM(B5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="beginsWith" dxfId="14" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="9" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="8" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="10">
       <formula>LEN(TRIM(B6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A7,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A7,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
-      <formula>LEN(TRIM(B7))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEF39D-E984-C449-9030-77DFE4612593}">
-  <dimension ref="A1:AAA24"/>
-  <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
-  <cols>
-    <col min="1" max="1" width="34" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="77.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:703">
-      <c r="A1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="HA1" s="6"/>
-      <c r="AAA1" s="6"/>
-    </row>
-    <row r="2" spans="1:703">
-      <c r="A2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="HA2" s="6"/>
-      <c r="AAA2" s="6"/>
-    </row>
-    <row r="3" spans="1:703">
-      <c r="A3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="HA3" s="6"/>
-      <c r="AAA3" s="6"/>
-    </row>
-    <row r="4" spans="1:703">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="7"/>
-      <c r="HA4" s="4"/>
-      <c r="AAA4" s="5"/>
-    </row>
-    <row r="5" spans="1:703">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="7"/>
-      <c r="HA5" s="4"/>
-      <c r="AAA5" s="5"/>
-    </row>
-    <row r="6" spans="1:703">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="7"/>
-      <c r="HA6" s="4"/>
-      <c r="AAA6" s="5"/>
-    </row>
-    <row r="7" spans="1:703">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="7"/>
-      <c r="HA7" s="4"/>
-      <c r="AAA7" s="5"/>
-    </row>
-    <row r="8" spans="1:703">
-      <c r="A8" s="12"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="7"/>
-      <c r="HA8" s="4"/>
-      <c r="AAA8" s="5"/>
-    </row>
-    <row r="9" spans="1:703">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="7"/>
-      <c r="HA9" s="4"/>
-      <c r="AAA9" s="5"/>
-    </row>
-    <row r="10" spans="1:703">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="7"/>
-      <c r="HA10" s="4"/>
-      <c r="AAA10" s="5"/>
-    </row>
-    <row r="11" spans="1:703">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:703">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:703">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:703">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:703">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:703">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
-      <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
-      <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="5">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
+      <formula>LEN(TRIM(B7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test artifacts for database automation updated
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-02.data.xlsx
+++ b/artifact/data/rdbms-02.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D898C3-275A-F047-B7D1-BEEC53E105E1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0222E2B3-E700-3643-9621-7956DDAD912E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="10280" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>true</t>
   </si>
@@ -422,9 +422,6 @@
       <t>'
 ORDER BY REP_NAME, CUSTOMER_NAME;</t>
     </r>
-  </si>
-  <si>
-    <t>media type</t>
   </si>
   <si>
     <t>${mediatype}</t>
@@ -557,7 +554,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -591,7 +588,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -602,7 +598,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="85">
     <dxf>
       <font>
         <b val="0"/>
@@ -1153,43 +1149,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1580,6 +1539,43 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1608,29 +1604,38 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1988,9 +1993,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA13"/>
+  <dimension ref="A1:AAA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2002,7 +2009,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2010,7 +2017,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -2018,7 +2025,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -2026,7 +2033,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -2034,7 +2041,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -2042,7 +2049,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -2050,91 +2057,68 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="83" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+  <conditionalFormatting sqref="A10:A1048576 A1:A7">
+    <cfRule type="beginsWith" dxfId="84" priority="13" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="82" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="83" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="81" priority="7" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="15" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B7 B13:B1048576">
-    <cfRule type="expression" dxfId="80" priority="8" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B7 B10:B1048576">
+    <cfRule type="expression" dxfId="81" priority="16" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="79" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="17">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="78" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="A9">
+    <cfRule type="beginsWith" dxfId="79" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A9,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="78" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A9,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="77" priority="6" stopIfTrue="1">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="76" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="77" priority="4">
-      <formula>LEN(TRIM(B12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10:B11">
-    <cfRule type="expression" dxfId="76" priority="1" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="75" priority="2">
-      <formula>LEN(TRIM(B10))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="75" priority="8">
+      <formula>LEN(TRIM(B9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="beginsWith" dxfId="74" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A8,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="73" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A8,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="72" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2146,7 +2130,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC08D69-8887-4444-B785-D23953AF8585}">
   <dimension ref="A1:AAA3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2179,21 +2165,21 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="74" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="71" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="73" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="70" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="72" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="71" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="70" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2206,7 +2192,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D8DAAF-5FA2-3F45-9587-0BF4D1FC794A}">
   <dimension ref="A1:AAA3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2239,21 +2227,21 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="69" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="66" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="68" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="65" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="67" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="66" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="65" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2266,7 +2254,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A45AD1-9E5F-1D4C-908D-A0E650034FFE}">
   <dimension ref="A1:AAA7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2331,59 +2321,59 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A4 A7">
-    <cfRule type="beginsWith" dxfId="64" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="61" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="63" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="60" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="62" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B4 B7">
-    <cfRule type="expression" dxfId="61" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="60" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="20">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="beginsWith" dxfId="59" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="56" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A5,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="58" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="55" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A5,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="57" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="56" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="55" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="10">
       <formula>LEN(TRIM(B5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="beginsWith" dxfId="54" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="51" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="53" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="50" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="52" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="51" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="50" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="5">
       <formula>LEN(TRIM(B6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2394,9 +2384,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5615C66-E964-DF4A-B5AC-E5F1CF42C1A0}">
-  <dimension ref="A1:AAA9"/>
+  <dimension ref="A1:AAA12"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2462,56 +2454,38 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A1:A4 A9:A1048576">
-    <cfRule type="beginsWith" dxfId="49" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+  <conditionalFormatting sqref="A1:A4 A10:A1048576">
+    <cfRule type="beginsWith" dxfId="46" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="45" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="47" priority="28" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B4 B9:B1048576">
-    <cfRule type="expression" dxfId="46" priority="29" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B4 B10:B1048576">
+    <cfRule type="expression" dxfId="43" priority="29" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="45" priority="30">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="30">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="beginsWith" dxfId="44" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
-      <formula>LEFT(A8,LEN("sentry.scope."))="sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="43" priority="22" stopIfTrue="1" operator="beginsWith" text="sentry.">
-      <formula>LEFT(A8,LEN("sentry."))="sentry."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="42" priority="23" stopIfTrue="1">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
+  <conditionalFormatting sqref="B12">
     <cfRule type="expression" dxfId="41" priority="24" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="40" priority="25">
-      <formula>LEN(TRIM(B8))&gt;0</formula>
+      <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
@@ -2580,7 +2554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36E0F6B-8C25-A04E-A958-58437CE8DA7B}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
### General - fixed internal logic to handle the insertion of Excel rows that avoids the infamous "unreadable content" error. The   underlying bug (in POI) is documented here https://bz.apache.org/bugzilla/show_bug.cgi?id=57423 - enhance BaseCommand.addLinkToOutputFile() for great reusability.
#### [rdbms commands](../commands/rdbms/index)
- [rdbms &raquo; `saveResults(db,sqls,outputDir)`](../commands/rdbms/saveResults(db,sqls,outputDir)): **NEW** command
  to execute a series of queries and save the results to CSV files.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-02.data.xlsx
+++ b/artifact/data/rdbms-02.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10422"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0222E2B3-E700-3643-9621-7956DDAD912E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85BBDF3-5B55-AD49-8B7A-5D0DF288A53F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="10280" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9140" yWindow="-20560" windowWidth="33600" windowHeight="10280" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t>true</t>
   </si>
@@ -446,6 +446,12 @@
   </si>
   <si>
     <t>nexial.verbose</t>
+  </si>
+  <si>
+    <t>customers SQL file</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/rdbms-02-queries-to-csv.sql</t>
   </si>
 </sst>
 </file>
@@ -2552,10 +2558,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36E0F6B-8C25-A04E-A958-58437CE8DA7B}">
-  <dimension ref="A1:AAA10"/>
+  <dimension ref="A1:AAA11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -2639,8 +2645,20 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>

</xml_diff>